<commit_message>
Add driver_move package for tests. Add battery_module in driver hardware.
</commit_message>
<xml_diff>
--- a/hardware/misc/Battery_function.xlsx
+++ b/hardware/misc/Battery_function.xlsx
@@ -35,11 +35,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -55,6 +56,17 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,7 +172,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF004586"/>
@@ -214,6 +226,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -225,7 +238,7 @@
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="004586"/>
+                  <a:srgbClr val="ff420e"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -441,17 +454,17 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="67585851"/>
-        <c:axId val="41393807"/>
+        <c:axId val="82241366"/>
+        <c:axId val="8828092"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67585851"/>
+        <c:axId val="82241366"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -480,12 +493,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41393807"/>
+        <c:crossAx val="8828092"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41393807"/>
+        <c:axId val="8828092"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -500,7 +513,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -529,7 +542,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67585851"/>
+        <c:crossAx val="82241366"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -576,10 +589,10 @@
       <xdr:rowOff>141120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>483120</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>701640</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -587,8 +600,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2851200" y="466200"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="2813040" y="466200"/>
+        <a:ext cx="6689520" cy="4390920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -608,13 +621,13 @@
   </sheetPr>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>